<commit_message>
Criação da regra de negócio
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://redesignconsultorialtda-my.sharepoint.com/personal/daniel_philipi_redesignconsultoria_com_br/Documents/Área de Trabalho/Redesign/Exercício L3/Exercicio_UiPath_L3_Lite/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{684B2F63-4E27-4776-B188-0B474BF02F7D}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32BD2B81-A267-4928-8D48-F3BAE2AD7C6B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -159,9 +159,6 @@
     <t>Exercicio_UiPath_L3Lite</t>
   </si>
   <si>
-    <t>Nome_Empresa</t>
-  </si>
-  <si>
     <t>EmpresaFake</t>
   </si>
   <si>
@@ -175,6 +172,9 @@
   </si>
   <si>
     <t>Nome da empresa que será usado no preenchimento de notas</t>
+  </si>
+  <si>
+    <t>NomeEmpresa</t>
   </si>
 </sst>
 </file>
@@ -258,6 +258,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -560,7 +564,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -610,7 +614,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -621,7 +625,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
@@ -642,13 +646,13 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
         <v>44</v>
       </c>
-      <c r="B7" t="s">
-        <v>45</v>
-      </c>
       <c r="C7" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1829,7 +1833,7 @@
         <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>41</v>

</xml_diff>